<commit_message>
Lisätty ammuntaetäisyys, jokaisen kierroksen jälkeen syötetään tulokset -KV
</commit_message>
<xml_diff>
--- a/AmpuminenR1/Ajankäytönseurantagit.xlsx
+++ b/AmpuminenR1/Ajankäytönseurantagit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\inkak\Documents\Ohjelmistokehitys\Inkan gitit\AmpuminenR1\AmpuminenR1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lahde\OneDrive\Tiedostot\Gitit\AmpuminenR1\AmpuminenR1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1F4B4B9-4DED-4EFA-93A8-E303FE88811B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D607B61-C32D-42F0-AFAD-7C2943ADFF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9A2652D0-B9C0-4C5B-994F-291FBF012228}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="20">
   <si>
     <t>Ajankäytönseuranta</t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>Luento, Git Bashin ongelmien korjaus, Nano</t>
+  </si>
+  <si>
+    <t>Ohjelman aloitus</t>
+  </si>
+  <si>
+    <t>Ohjelman muokkausta</t>
   </si>
 </sst>
 </file>
@@ -340,9 +346,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 -teema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -380,7 +386,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -486,7 +492,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -628,7 +634,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -638,38 +644,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35986E9F-C3CA-4760-84FC-72F9332BEB4A}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="D8" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="49.42578125" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="49.44140625" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.33203125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" customWidth="1"/>
-    <col min="10" max="10" width="52.28515625" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.42578125" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="27.42578125" customWidth="1"/>
-    <col min="15" max="15" width="49.5703125" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" customWidth="1"/>
-    <col min="19" max="19" width="25.140625" customWidth="1"/>
-    <col min="20" max="20" width="51.28515625" customWidth="1"/>
+    <col min="9" max="9" width="25.109375" customWidth="1"/>
+    <col min="10" max="10" width="52.33203125" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.44140625" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" customWidth="1"/>
+    <col min="14" max="14" width="27.44140625" customWidth="1"/>
+    <col min="15" max="15" width="49.5546875" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" customWidth="1"/>
+    <col min="19" max="19" width="25.109375" customWidth="1"/>
+    <col min="20" max="20" width="51.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C2" s="24" t="s">
         <v>1</v>
       </c>
@@ -707,7 +713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="33" t="s">
         <v>4</v>
       </c>
@@ -757,7 +763,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C4" s="25">
         <v>45321</v>
       </c>
@@ -795,7 +801,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C5" s="20">
         <v>45323</v>
       </c>
@@ -833,7 +839,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C6" s="15">
         <v>45327</v>
       </c>
@@ -871,7 +877,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C7" s="15">
         <v>45328</v>
       </c>
@@ -903,7 +909,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C8" s="15">
         <v>45331</v>
       </c>
@@ -935,7 +941,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="18"/>
@@ -951,11 +957,17 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
       <c r="O9" s="18"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="18"/>
-    </row>
-    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R9" s="37">
+        <v>45333</v>
+      </c>
+      <c r="S9" s="11">
+        <v>3</v>
+      </c>
+      <c r="T9" s="32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="18"/>
@@ -965,11 +977,17 @@
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
       <c r="O10" s="18"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="18"/>
-    </row>
-    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R10" s="37">
+        <v>45334</v>
+      </c>
+      <c r="S10" s="11">
+        <v>2</v>
+      </c>
+      <c r="T10" s="32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="18"/>
@@ -983,7 +1001,7 @@
       <c r="S11" s="11"/>
       <c r="T11" s="18"/>
     </row>
-    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="18"/>
@@ -997,7 +1015,7 @@
       <c r="S12" s="11"/>
       <c r="T12" s="18"/>
     </row>
-    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="18"/>
@@ -1011,7 +1029,7 @@
       <c r="S13" s="11"/>
       <c r="T13" s="18"/>
     </row>
-    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="18"/>
@@ -1025,7 +1043,7 @@
       <c r="S14" s="11"/>
       <c r="T14" s="18"/>
     </row>
-    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="18"/>
@@ -1039,7 +1057,7 @@
       <c r="S15" s="11"/>
       <c r="T15" s="18"/>
     </row>
-    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="18"/>
@@ -1053,7 +1071,7 @@
       <c r="S16" s="11"/>
       <c r="T16" s="18"/>
     </row>
-    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="18"/>
@@ -1067,7 +1085,7 @@
       <c r="S17" s="11"/>
       <c r="T17" s="18"/>
     </row>
-    <row r="18" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="18"/>
@@ -1081,7 +1099,7 @@
       <c r="S18" s="11"/>
       <c r="T18" s="18"/>
     </row>
-    <row r="19" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="18"/>
@@ -1095,7 +1113,7 @@
       <c r="S19" s="11"/>
       <c r="T19" s="18"/>
     </row>
-    <row r="20" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="18"/>
@@ -1109,7 +1127,7 @@
       <c r="S20" s="11"/>
       <c r="T20" s="18"/>
     </row>
-    <row r="21" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="18"/>
@@ -1123,7 +1141,7 @@
       <c r="S21" s="11"/>
       <c r="T21" s="18"/>
     </row>
-    <row r="22" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="24.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="18"/>
@@ -1137,7 +1155,7 @@
       <c r="S22" s="11"/>
       <c r="T22" s="18"/>
     </row>
-    <row r="23" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="18"/>
@@ -1151,7 +1169,7 @@
       <c r="S23" s="11"/>
       <c r="T23" s="18"/>
     </row>
-    <row r="24" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="18"/>
@@ -1165,7 +1183,7 @@
       <c r="S24" s="11"/>
       <c r="T24" s="18"/>
     </row>
-    <row r="25" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>14</v>
       </c>
@@ -1190,7 +1208,7 @@
       <c r="R25" s="11"/>
       <c r="S25" s="13">
         <f>SUM(S3:S23)</f>
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="T25" s="18"/>
     </row>
@@ -1200,9 +1218,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1350,19 +1371,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1386,9 +1403,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8476295D-41CE-4307-91AF-C4C5E867FE62}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{668CA308-F1BC-4E87-B54F-96008F032242}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>